<commit_message>
Updated to version 1.1
</commit_message>
<xml_diff>
--- a/Documentation/Rocket_Switch_Interface_BOM.xlsx
+++ b/Documentation/Rocket_Switch_Interface_BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://neilsquiresoc.sharepoint.com/sites/MMC-RD/Shared Documents/RD 22-08 Rocket Switch Interface/Documentation/Working_Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Milad\Development\NSS\MMC\Github_Projects\Rocket-Switch-Interface\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{0B8E08CA-0295-4D81-99D4-E8041F22A9F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0602C9DF-9EFB-4658-A1FC-D83E0CE3D998}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D35422E1-72EF-4D6E-ABF2-A5DC98D642FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,6 +45,141 @@
     <t>Total filament (g)</t>
   </si>
   <si>
+    <t>Commercial Parts:</t>
+  </si>
+  <si>
+    <t>Part type (Electrical. Mechanical, Sanitization, ect)</t>
+  </si>
+  <si>
+    <t>Part Name</t>
+  </si>
+  <si>
+    <t>Quantity Needed</t>
+  </si>
+  <si>
+    <t>Pkg Quantity</t>
+  </si>
+  <si>
+    <t>Price per package</t>
+  </si>
+  <si>
+    <t>Price per Unit</t>
+  </si>
+  <si>
+    <t>Price for qty needed</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>3D Printed Parts                                                                                     ESTIMATED PRICING USING 1KG ROLL COST:</t>
+  </si>
+  <si>
+    <t>Part</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>TOTAL Mass (g)</t>
+  </si>
+  <si>
+    <t>Estimated Price</t>
+  </si>
+  <si>
+    <t>Print Time (Min)</t>
+  </si>
+  <si>
+    <t>Total Print Cost:</t>
+  </si>
+  <si>
+    <t>Tools for Assembly</t>
+  </si>
+  <si>
+    <t>Alternatives (if there are other sources for some parts link them below)</t>
+  </si>
+  <si>
+    <t>Part and description</t>
+  </si>
+  <si>
+    <t>Electrical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adafruit Rotary Trinkey </t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/cui-devices/SJ-43514/368146</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/stackpole-electronics-inc/CFM14JT4K70/1742213</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.7 kOhms 1/4W Through Hole Resistor </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SJ-43514 3.5mm Jack Stereo </t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/adafruit-industries-llc/4964/14307384</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/dialight/51513030250F/4965201</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Light Pipe </t>
+  </si>
+  <si>
+    <t>Soldering iron</t>
+  </si>
+  <si>
+    <t>Rocket-Switch-Interface-Bottom-Case</t>
+  </si>
+  <si>
+    <t>Rocket-Switch-Interface-Top-Case</t>
+  </si>
+  <si>
+    <t>Rocket-Switch-Interface-Jig</t>
+  </si>
+  <si>
+    <t>https://github.com/makersmakingchange/Rocket-Switch-Interface/tree/main/Build_Files/3D_Print_Files/STL/Rocket-Switch-Interface-Bottom-Case.stl</t>
+  </si>
+  <si>
+    <t>https://github.com/makersmakingchange/Rocket-Switch-Interface/tree/main/Build_Files/3D_Print_Files/STL/Rocket-Switch-Interface-Top-Case.stl</t>
+  </si>
+  <si>
+    <t>https://github.com/makersmakingchange/Rocket-Switch-Interface/tree/main/Build_Files/3D_Print_Files/STL/Rocket-Switch-Interface-Jig.stl</t>
+  </si>
+  <si>
+    <t>15% Infill</t>
+  </si>
+  <si>
+    <t>Part Label</t>
+  </si>
+  <si>
+    <t>R1,R2</t>
+  </si>
+  <si>
+    <t>SW1,SW2</t>
+  </si>
+  <si>
+    <t>Date Created: 10/28/2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alternate Links </t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/apm-hexseal/RM3X8MM-2701/3712297</t>
+  </si>
+  <si>
+    <t>M3 8MM Pan Head Machine Screw Phillip</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/w%C3%BCrth-elektronik/97790803111/10056388</t>
+  </si>
+  <si>
+    <t>Device:  Rocket-Switch-Interface V1.1</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Version: </t>
     </r>
@@ -58,143 +193,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>V1.0</t>
+      <t>V1.1</t>
     </r>
-  </si>
-  <si>
-    <t>Commercial Parts:</t>
-  </si>
-  <si>
-    <t>Part type (Electrical. Mechanical, Sanitization, ect)</t>
-  </si>
-  <si>
-    <t>Part Name</t>
-  </si>
-  <si>
-    <t>Quantity Needed</t>
-  </si>
-  <si>
-    <t>Pkg Quantity</t>
-  </si>
-  <si>
-    <t>Price per package</t>
-  </si>
-  <si>
-    <t>Price per Unit</t>
-  </si>
-  <si>
-    <t>Price for qty needed</t>
-  </si>
-  <si>
-    <t>Link</t>
-  </si>
-  <si>
-    <t>3D Printed Parts                                                                                     ESTIMATED PRICING USING 1KG ROLL COST:</t>
-  </si>
-  <si>
-    <t>Part</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>TOTAL Mass (g)</t>
-  </si>
-  <si>
-    <t>Estimated Price</t>
-  </si>
-  <si>
-    <t>Print Time (Min)</t>
-  </si>
-  <si>
-    <t>Total Print Cost:</t>
-  </si>
-  <si>
-    <t>Tools for Assembly</t>
-  </si>
-  <si>
-    <t>Alternatives (if there are other sources for some parts link them below)</t>
-  </si>
-  <si>
-    <t>Part and description</t>
-  </si>
-  <si>
-    <t>Electrical</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adafruit Rotary Trinkey </t>
-  </si>
-  <si>
-    <t>https://www.digikey.ca/en/products/detail/cui-devices/SJ-43514/368146</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ca/en/products/detail/stackpole-electronics-inc/CFM14JT4K70/1742213</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.7 kOhms 1/4W Through Hole Resistor </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SJ-43514 3.5mm Jack Stereo </t>
-  </si>
-  <si>
-    <t>https://www.digikey.ca/en/products/detail/adafruit-industries-llc/4964/14307384</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ca/en/products/detail/dialight/51513030250F/4965201</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Light Pipe </t>
-  </si>
-  <si>
-    <t>Soldering iron</t>
-  </si>
-  <si>
-    <t>Rocket-Switch-Interface-Bottom-Case</t>
-  </si>
-  <si>
-    <t>Rocket-Switch-Interface-Top-Case</t>
-  </si>
-  <si>
-    <t>Rocket-Switch-Interface-Jig</t>
-  </si>
-  <si>
-    <t>https://github.com/makersmakingchange/Rocket-Switch-Interface/tree/main/Build_Files/3D_Print_Files/STL/Rocket-Switch-Interface-Bottom-Case.stl</t>
-  </si>
-  <si>
-    <t>https://github.com/makersmakingchange/Rocket-Switch-Interface/tree/main/Build_Files/3D_Print_Files/STL/Rocket-Switch-Interface-Top-Case.stl</t>
-  </si>
-  <si>
-    <t>https://github.com/makersmakingchange/Rocket-Switch-Interface/tree/main/Build_Files/3D_Print_Files/STL/Rocket-Switch-Interface-Jig.stl</t>
-  </si>
-  <si>
-    <t>15% Infill</t>
-  </si>
-  <si>
-    <t>Part Label</t>
-  </si>
-  <si>
-    <t>R1,R2</t>
-  </si>
-  <si>
-    <t>SW1,SW2</t>
-  </si>
-  <si>
-    <t>Date Created: 10/28/2022</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ca/en/products/detail/w%C3%BCrth-elektronik/97790603111/10056387</t>
-  </si>
-  <si>
-    <t>M3 6MM Pan Head Machine Screw Phillip</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alternate Links </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.ca/en/products/detail/apm-hexseal/RM3X6MM-2701/612968 </t>
-  </si>
-  <si>
-    <t>Device:  Rocket-Switch-Interface V1.0</t>
   </si>
 </sst>
 </file>
@@ -811,8 +811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -833,7 +833,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="35.25" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
@@ -847,70 +847,70 @@
     </row>
     <row r="2" spans="1:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="5">
         <f>SUM(H5:H11)+F18</f>
-        <v>15.341750000000001</v>
+        <v>15.316250000000002</v>
       </c>
       <c r="E2" s="23">
         <f>SUM(G13:G17)/60</f>
-        <v>0.81666666666666665</v>
+        <v>1.0166666666666666</v>
       </c>
       <c r="F2" s="6">
         <f>SUM(E13:E17)</f>
-        <v>8.8699999999999992</v>
+        <v>8.65</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="C4" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="16" t="s">
+      <c r="E4" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="F4" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="G4" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="H4" s="16" t="s">
         <v>10</v>
-      </c>
-      <c r="H4" s="16" t="s">
-        <v>11</v>
       </c>
       <c r="I4" s="16"/>
       <c r="J4" s="16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="L4" s="7"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="29" t="s">
         <v>23</v>
-      </c>
-      <c r="B5" s="29" t="s">
-        <v>24</v>
       </c>
       <c r="C5" s="29"/>
       <c r="D5" s="29">
@@ -930,18 +930,18 @@
         <v>9.73</v>
       </c>
       <c r="J5" s="31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D6" s="29">
         <v>2</v>
@@ -960,18 +960,18 @@
         <v>2.96</v>
       </c>
       <c r="J6" s="31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D7" s="29">
         <v>2</v>
@@ -990,15 +990,15 @@
         <v>0.3</v>
       </c>
       <c r="J7" s="31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C8" s="29"/>
       <c r="D8" s="29">
@@ -1018,12 +1018,12 @@
         <v>1.7</v>
       </c>
       <c r="J8" s="31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="29" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="29" t="s">
         <v>45</v>
@@ -1036,20 +1036,20 @@
         <v>1</v>
       </c>
       <c r="F9" s="30">
-        <v>0.43</v>
+        <v>0.41</v>
       </c>
       <c r="G9" s="30">
-        <v>0.43</v>
+        <v>0.41</v>
       </c>
       <c r="H9" s="17">
         <f>G9*D9</f>
-        <v>0.43</v>
+        <v>0.41</v>
       </c>
       <c r="J9" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="K9" s="8" t="s">
         <v>44</v>
-      </c>
-      <c r="K9" s="8" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1059,7 +1059,7 @@
     </row>
     <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" s="33">
         <v>25</v>
@@ -1072,98 +1072,98 @@
     </row>
     <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="25" t="s">
         <v>14</v>
-      </c>
-      <c r="B12" s="25" t="s">
-        <v>15</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E12" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="G12" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="G12" s="7" t="s">
-        <v>18</v>
-      </c>
       <c r="H12" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13">
-        <v>4.53</v>
+        <v>4.4800000000000004</v>
       </c>
       <c r="F13" s="17">
         <f>(E13/1000)*$B$11</f>
-        <v>0.11325</v>
+        <v>0.11200000000000002</v>
       </c>
       <c r="G13">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
       <c r="E14">
-        <v>3.83</v>
+        <v>3.64</v>
       </c>
       <c r="F14" s="17">
         <f t="shared" ref="F14:F17" si="0">(E14/1000)*$B$11</f>
-        <v>9.5750000000000002E-2</v>
+        <v>9.0999999999999998E-2</v>
       </c>
       <c r="G14">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="E15">
-        <v>0.51</v>
+        <v>0.53</v>
       </c>
       <c r="F15" s="17">
         <f t="shared" si="0"/>
-        <v>1.2750000000000001E-2</v>
+        <v>1.325E-2</v>
       </c>
       <c r="G15">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -1183,17 +1183,17 @@
     <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="12"/>
       <c r="E18" s="19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F18" s="20">
         <f>SUM(F13:F17)</f>
-        <v>0.22175000000000003</v>
+        <v>0.21625000000000003</v>
       </c>
       <c r="H18" s="13"/>
     </row>
     <row r="19" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
@@ -1210,13 +1210,13 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B26" s="32"/>
       <c r="C26" s="11"/>
@@ -1233,10 +1233,10 @@
     </row>
     <row r="27" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B27" s="28" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1257,14 +1257,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cf9f6c1f-8ad0-4eb8-bb2b-fb0b622a341e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="72c39c84-b0a3-45a2-a38c-ff46bb47f11f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1505,29 +1503,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cf9f6c1f-8ad0-4eb8-bb2b-fb0b622a341e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="72c39c84-b0a3-45a2-a38c-ff46bb47f11f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4958292-C6C4-482B-887A-6CF9FB19AB74}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4740145F-09D2-466B-B9A2-2798696B0ADF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="1ccc884c-acc6-4907-b9d9-a5a76f4fb80e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="e4aa5b0e-c599-4492-a04c-87c1e111489c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="cf9f6c1f-8ad0-4eb8-bb2b-fb0b622a341e"/>
-    <ds:schemaRef ds:uri="72c39c84-b0a3-45a2-a38c-ff46bb47f11f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1552,9 +1541,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4740145F-09D2-466B-B9A2-2798696B0ADF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4958292-C6C4-482B-887A-6CF9FB19AB74}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="1ccc884c-acc6-4907-b9d9-a5a76f4fb80e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="e4aa5b0e-c599-4492-a04c-87c1e111489c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="cf9f6c1f-8ad0-4eb8-bb2b-fb0b622a341e"/>
+    <ds:schemaRef ds:uri="72c39c84-b0a3-45a2-a38c-ff46bb47f11f"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>